<commit_message>
Update file containing menu import test data
Add test file for menu import functionality.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: e9bfec2c-7174-45ec-80c1-6a86056a427c
Replit-Commit-Checkpoint-Type: intermediate_checkpoint
Replit-Commit-Event-Id: b966691d-2b44-4e3b-b9cd-b9e62d46d311
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/b0c93d92-bfba-41ae-8ac6-8fbd66f218e1/e9bfec2c-7174-45ec-80c1-6a86056a427c/gGNIRwg
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/test_menu_import.xlsx
+++ b/test_menu_import.xlsx
@@ -436,7 +436,7 @@
         <v>250</v>
       </c>
       <c r="D2" t="str">
-        <v>starters</v>
+        <v>american-irish-whiskey</v>
       </c>
       <c r="E2" t="str">
         <v>TRUE</v>
@@ -459,7 +459,7 @@
         <v>150 | 250 | 350</v>
       </c>
       <c r="D3" t="str">
-        <v>combos</v>
+        <v>asian-mains</v>
       </c>
       <c r="E3" t="str">
         <v>TRUE</v>

</xml_diff>